<commit_message>
added Artix power sheet, updated power consumption sheet.
</commit_message>
<xml_diff>
--- a/SIM_CALC/power consumption.xlsx
+++ b/SIM_CALC/power consumption.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michal\Desktop\Projekty\ARTIQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\DESIGNS\MTCA projects\SINARA\SIM_CALC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11070" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metlino" sheetId="1" r:id="rId1"/>
     <sheet name="Sayma_AMC" sheetId="2" r:id="rId2"/>
     <sheet name="Sayma_RTM" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="74">
   <si>
     <t>3V3MP</t>
   </si>
@@ -227,12 +227,33 @@
   </si>
   <si>
     <t>Voltage [V]</t>
+  </si>
+  <si>
+    <t>clock mezzanine</t>
+  </si>
+  <si>
+    <t>derived from</t>
+  </si>
+  <si>
+    <t>AMC MP</t>
+  </si>
+  <si>
+    <t>AMC +12</t>
+  </si>
+  <si>
+    <t>RTM + 12</t>
+  </si>
+  <si>
+    <t>RTM MP</t>
+  </si>
+  <si>
+    <t>ADT7420</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -305,7 +326,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1181,10 +1202,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,479 +1216,511 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
       <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3">
-        <v>1E-4</v>
-      </c>
-      <c r="D3">
-        <v>1E-4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C4">
-        <v>2E-3</v>
+        <v>1E-4</v>
+      </c>
+      <c r="D4">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>0.08</v>
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6">
-        <v>0.5</v>
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0.08</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>0.1</v>
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>3.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>1E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12">
-        <v>0.8</v>
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>0.1</v>
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>0.8</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="C14">
         <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15">
-        <v>2E-3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16">
-        <v>0.2</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20">
-        <v>0.06</v>
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>0.3</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21">
-        <v>0.04</v>
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>0.06</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22">
-        <v>1.7</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>0.6</v>
-      </c>
-      <c r="H22">
-        <v>3.04</v>
-      </c>
-      <c r="I22">
-        <v>3.1E-2</v>
-      </c>
-      <c r="J22">
-        <v>9.7850000000000001</v>
+        <v>25</v>
+      </c>
+      <c r="D22">
+        <v>0.04</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="E23">
+        <v>1.7</v>
       </c>
       <c r="F23">
-        <f>G25</f>
+        <v>1</v>
+      </c>
+      <c r="G23">
         <v>0.6</v>
+      </c>
+      <c r="H23">
+        <v>3.04</v>
+      </c>
+      <c r="I23">
+        <v>3.1E-2</v>
+      </c>
+      <c r="J23">
+        <v>9.7850000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24">
+        <f>G26</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="D24">
-        <f>I25</f>
+      <c r="D25">
+        <f>I26</f>
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="4">
-        <f>SUM(B3:B22)</f>
-        <v>0</v>
-      </c>
-      <c r="C25" s="4">
-        <f t="shared" ref="C25:J25" si="0">SUM(C3:C24)</f>
+      <c r="B26" s="4">
+        <f>SUM(B4:B23)</f>
+        <v>0.36</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" ref="C26:J26" si="0">SUM(C4:C25)</f>
         <v>0.21010000000000001</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D26" s="4">
         <f t="shared" si="0"/>
-        <v>2.2631000000000001</v>
-      </c>
-      <c r="E25" s="4">
+        <v>1.9831000000000001</v>
+      </c>
+      <c r="E26" s="4">
         <f t="shared" si="0"/>
-        <v>1.78</v>
-      </c>
-      <c r="F25" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="F26" s="4">
         <f t="shared" si="0"/>
         <v>3.1</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G26" s="4">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H26" s="4">
         <f t="shared" si="0"/>
         <v>3.04</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I26" s="4">
         <f t="shared" si="0"/>
         <v>3.1E-2</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J26" s="4">
         <f t="shared" si="0"/>
         <v>9.7850000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="D26" s="5">
-        <v>3.2</v>
-      </c>
-      <c r="E26" s="5">
-        <v>3.2</v>
-      </c>
-      <c r="F26" s="5">
-        <v>3.2</v>
-      </c>
-      <c r="G26" s="5">
-        <v>3</v>
-      </c>
-      <c r="H26" s="5">
-        <v>3.2</v>
-      </c>
-      <c r="I26" s="5">
-        <v>3</v>
-      </c>
-      <c r="J26" s="5">
-        <v>20</v>
-      </c>
-    </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="E27" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="F27" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="G27" s="5">
+        <v>3</v>
+      </c>
+      <c r="H27" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="I27" s="5">
+        <v>3</v>
+      </c>
+      <c r="J27" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>66</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>5</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>3.3</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>3.3</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <v>1.8</v>
       </c>
-      <c r="F27">
+      <c r="F28">
         <v>1.5</v>
       </c>
-      <c r="G27">
+      <c r="G28">
         <v>1.2</v>
       </c>
-      <c r="H27">
+      <c r="H28">
         <v>1</v>
       </c>
-      <c r="I27">
+      <c r="I28">
         <v>0.95</v>
       </c>
-      <c r="J27">
+      <c r="J28">
         <v>0.9</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="L28" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="12">
-        <f>B27*B25</f>
-        <v>0</v>
-      </c>
-      <c r="C28" s="12">
-        <f>C27*C25</f>
+      <c r="B29" s="12">
+        <f>B28*B26</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="C29" s="12">
+        <f>C28*C26</f>
         <v>0.69333</v>
       </c>
-      <c r="D28" s="12">
-        <f t="shared" ref="D28:J28" si="1">D27*D25</f>
-        <v>7.4682300000000001</v>
-      </c>
-      <c r="E28" s="12">
+      <c r="D29" s="12">
+        <f t="shared" ref="D29:J29" si="1">D28*D26</f>
+        <v>6.5442299999999998</v>
+      </c>
+      <c r="E29" s="12">
         <f t="shared" si="1"/>
-        <v>3.2040000000000002</v>
-      </c>
-      <c r="F28" s="12">
+        <v>3.06</v>
+      </c>
+      <c r="F29" s="12">
         <f t="shared" si="1"/>
         <v>4.6500000000000004</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G29" s="12">
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H29" s="12">
         <f t="shared" si="1"/>
         <v>3.04</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I29" s="12">
         <f t="shared" si="1"/>
         <v>2.9449999999999997E-2</v>
       </c>
-      <c r="J28" s="12">
+      <c r="J29" s="12">
         <f t="shared" si="1"/>
         <v>8.8064999999999998</v>
       </c>
-      <c r="L28" s="3">
-        <f>SUM(E28:J28)</f>
-        <v>20.449950000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="L29" s="3">
+        <f>SUM(E29:J29)</f>
+        <v>20.305950000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>43</v>
       </c>
-      <c r="C29">
+      <c r="C30">
         <v>1</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>0.85</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <v>0.85</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <v>0.85</v>
       </c>
-      <c r="G29">
+      <c r="G30">
         <v>1</v>
       </c>
-      <c r="H29">
+      <c r="H30">
         <v>0.85</v>
       </c>
-      <c r="I29">
+      <c r="I30">
         <v>1</v>
       </c>
-      <c r="J29">
+      <c r="J30">
         <v>0.9</v>
       </c>
-      <c r="L29" s="11" t="s">
+      <c r="L30" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13" t="s">
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14">
-        <f>C28/C29</f>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14">
+        <f>C29/C30</f>
         <v>0.69333</v>
       </c>
-      <c r="D30" s="14">
-        <f t="shared" ref="D30:J30" si="2">D28/D29</f>
-        <v>8.7861529411764714</v>
-      </c>
-      <c r="E30" s="14">
+      <c r="D31" s="14">
+        <f t="shared" ref="D31:J31" si="2">D29/D30</f>
+        <v>7.6990941176470589</v>
+      </c>
+      <c r="E31" s="14">
         <f t="shared" si="2"/>
-        <v>3.7694117647058825</v>
-      </c>
-      <c r="F30" s="14">
+        <v>3.6</v>
+      </c>
+      <c r="F31" s="14">
         <f t="shared" si="2"/>
         <v>5.4705882352941186</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G31" s="14">
         <f t="shared" si="2"/>
         <v>0.72</v>
       </c>
-      <c r="H30" s="14">
+      <c r="H31" s="14">
         <f t="shared" si="2"/>
         <v>3.5764705882352943</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I31" s="14">
         <f t="shared" si="2"/>
         <v>2.9449999999999997E-2</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J31" s="15">
         <f t="shared" si="2"/>
         <v>9.7850000000000001</v>
       </c>
-      <c r="L30" s="10">
-        <f>SUM(C30:J30)</f>
-        <v>32.830403529411768</v>
+      <c r="L31" s="10">
+        <f>SUM(C31:J31)</f>
+        <v>31.573932941176473</v>
       </c>
     </row>
   </sheetData>
@@ -1678,10 +1731,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N28"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,6 +1745,47 @@
     <col min="14" max="14" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -1735,14 +1829,14 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="D4">
+      <c r="B4">
         <v>0.06</v>
       </c>
     </row>
@@ -1750,7 +1844,7 @@
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="D5">
+      <c r="B5">
         <v>0.3</v>
       </c>
     </row>
@@ -1775,427 +1869,454 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="D8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="K8">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9">
-        <v>2E-3</v>
+        <v>44</v>
+      </c>
+      <c r="D9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K9">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10">
-        <v>1E-3</v>
+        <v>45</v>
+      </c>
+      <c r="E10">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D12">
-        <v>5.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D13">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14">
-        <v>3.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15">
-        <v>2.1999999999999999E-2</v>
+        <v>49</v>
+      </c>
+      <c r="C15">
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="K16">
-        <v>1.2</v>
+        <v>50</v>
+      </c>
+      <c r="I16">
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="K17">
-        <v>0.1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="I18">
-        <v>0.26</v>
+        <v>53</v>
+      </c>
+      <c r="K18">
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="K19">
-        <v>0.5</v>
+        <v>59</v>
+      </c>
+      <c r="I19">
+        <v>0.26</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20">
-        <v>0.15</v>
-      </c>
-      <c r="E20">
+        <v>60</v>
+      </c>
+      <c r="K20">
         <v>0.5</v>
-      </c>
-      <c r="F20">
-        <v>0.5</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>0.03</v>
+      </c>
+      <c r="E21">
+        <v>0.5</v>
+      </c>
+      <c r="F21">
+        <v>0.5</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>62</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>4</v>
       </c>
-      <c r="H21">
+      <c r="H22">
         <v>0.4</v>
       </c>
-      <c r="I21">
+      <c r="I22">
         <v>6</v>
       </c>
-      <c r="L21">
+      <c r="L22">
         <v>0.8</v>
       </c>
-      <c r="M21">
+      <c r="M22">
         <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0.1</v>
+      </c>
+      <c r="I23">
+        <v>1.5</v>
+      </c>
+      <c r="L23">
+        <v>0.2</v>
+      </c>
+      <c r="M23">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="4">
-        <f t="shared" ref="B23:K23" si="0">SUM(B3:B22)</f>
-        <v>0</v>
-      </c>
-      <c r="C23" s="4">
+      <c r="B24" s="4">
+        <f t="shared" ref="B24:K24" si="0">SUM(B3:B23)</f>
+        <v>0.36</v>
+      </c>
+      <c r="C24" s="4">
         <f t="shared" si="0"/>
         <v>6.1000000000000006E-2</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D24" s="16">
         <f t="shared" si="0"/>
-        <v>4.62</v>
-      </c>
-      <c r="E23" s="4">
+        <v>5.0460000000000003</v>
+      </c>
+      <c r="E24" s="4">
         <f t="shared" si="0"/>
         <v>0.502</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F24" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G24" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H24" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H23" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="4">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="I23" s="4">
-        <f t="shared" si="0"/>
-        <v>6.282</v>
-      </c>
-      <c r="J23" s="4">
+        <v>7.782</v>
+      </c>
+      <c r="J24" s="4">
         <f t="shared" si="0"/>
         <v>3.4</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K24" s="4">
         <f t="shared" si="0"/>
         <v>3.2049999999999996</v>
       </c>
-      <c r="L23" s="4">
-        <f>SUM(L3:L22)</f>
-        <v>0.8</v>
-      </c>
-      <c r="M23" s="4">
-        <f>SUM(M3:M22)</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5">
-        <v>4</v>
-      </c>
-      <c r="E24" s="5">
-        <v>2</v>
-      </c>
-      <c r="F24" s="5">
-        <v>2</v>
-      </c>
-      <c r="G24" s="5">
-        <v>4</v>
-      </c>
-      <c r="H24" s="5">
-        <v>2</v>
-      </c>
-      <c r="I24" s="5">
-        <v>8</v>
-      </c>
-      <c r="J24">
-        <v>4</v>
-      </c>
-      <c r="K24">
-        <v>4</v>
-      </c>
-      <c r="L24" s="5">
+      <c r="L24" s="4">
+        <f>SUM(L3:L23)</f>
         <v>1</v>
       </c>
-      <c r="M24">
-        <v>1</v>
+      <c r="M24" s="4">
+        <f>SUM(M3:M23)</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25">
-        <v>5</v>
-      </c>
-      <c r="C25">
-        <v>3.3</v>
-      </c>
-      <c r="D25">
-        <v>3.3</v>
-      </c>
-      <c r="E25">
-        <v>1.8</v>
-      </c>
-      <c r="F25">
-        <v>1.2</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
+        <v>65</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5">
         <v>6</v>
       </c>
-      <c r="I25">
-        <v>6</v>
+      <c r="E25" s="5">
+        <v>2</v>
+      </c>
+      <c r="F25" s="5">
+        <v>2</v>
+      </c>
+      <c r="G25" s="5">
+        <v>4</v>
+      </c>
+      <c r="H25" s="5">
+        <v>2</v>
+      </c>
+      <c r="I25" s="5">
+        <v>8</v>
       </c>
       <c r="J25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K25">
         <v>4</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="5">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>3.3</v>
+      </c>
+      <c r="D26">
+        <v>3.3</v>
+      </c>
+      <c r="E26">
+        <v>1.8</v>
+      </c>
+      <c r="F26">
+        <v>1.2</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26">
         <v>12</v>
       </c>
-      <c r="M25">
+      <c r="M26">
         <v>12</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="N26" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="12">
-        <f>B25*B23</f>
-        <v>0</v>
-      </c>
-      <c r="C26" s="12">
-        <f>C25*C23</f>
+      <c r="B27" s="12">
+        <f>B26*B24</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="C27" s="12">
+        <f>C26*C24</f>
         <v>0.20130000000000001</v>
       </c>
-      <c r="D26" s="12">
-        <f t="shared" ref="D26:M26" si="1">D25*D23</f>
-        <v>15.245999999999999</v>
-      </c>
-      <c r="E26" s="12">
+      <c r="D27" s="12">
+        <f t="shared" ref="D27:M27" si="1">D26*D24</f>
+        <v>16.651800000000001</v>
+      </c>
+      <c r="E27" s="12">
         <f t="shared" si="1"/>
         <v>0.90360000000000007</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F27" s="12">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G27" s="12">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H26" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="H27" s="12">
         <f t="shared" si="1"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="I26" s="12">
+        <v>3</v>
+      </c>
+      <c r="I27" s="12">
         <f t="shared" si="1"/>
-        <v>37.692</v>
-      </c>
-      <c r="J26" s="12">
+        <v>46.692</v>
+      </c>
+      <c r="J27" s="12">
         <f t="shared" si="1"/>
         <v>6.8</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K27" s="12">
         <f t="shared" si="1"/>
         <v>12.819999999999999</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L27" s="12">
         <f t="shared" si="1"/>
-        <v>9.6000000000000014</v>
-      </c>
-      <c r="M26" s="12">
+        <v>12</v>
+      </c>
+      <c r="M27" s="12">
         <f t="shared" si="1"/>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="N26" s="3">
-        <f>SUM(D26:G26)</f>
-        <v>17.749600000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="N27" s="3">
+        <f>SUM(D27:G27)</f>
+        <v>19.655400000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>1</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>0.85</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <v>0.85</v>
       </c>
-      <c r="F27">
+      <c r="F28">
         <v>0.85</v>
       </c>
-      <c r="G27">
+      <c r="G28">
         <v>0.85</v>
       </c>
-      <c r="H27">
+      <c r="H28">
         <v>0.8</v>
       </c>
-      <c r="I27">
+      <c r="I28">
         <v>0.9</v>
       </c>
-      <c r="J27">
+      <c r="J28">
         <v>0.85</v>
       </c>
-      <c r="K27">
+      <c r="K28">
         <v>0.85</v>
       </c>
-      <c r="L27">
+      <c r="L28">
         <v>0.8</v>
       </c>
-      <c r="M27">
+      <c r="M28">
         <v>0.8</v>
       </c>
-      <c r="N27" s="11" t="s">
+      <c r="N28" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14">
-        <f>C26/C27</f>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14">
+        <f>C27/C28</f>
         <v>0.20130000000000001</v>
       </c>
-      <c r="D28" s="14">
-        <f t="shared" ref="D28:M28" si="2">D26/D27</f>
-        <v>17.936470588235292</v>
-      </c>
-      <c r="E28" s="14">
+      <c r="D29" s="14">
+        <f t="shared" ref="D29:M29" si="2">D27/D28</f>
+        <v>19.590352941176473</v>
+      </c>
+      <c r="E29" s="14">
         <f t="shared" si="2"/>
         <v>1.0630588235294118</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F29" s="14">
         <f t="shared" si="2"/>
         <v>0.70588235294117652</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G29" s="14">
         <f t="shared" si="2"/>
-        <v>1.1764705882352942</v>
-      </c>
-      <c r="H28" s="14">
+        <v>1.7647058823529411</v>
+      </c>
+      <c r="H29" s="14">
         <f t="shared" si="2"/>
-        <v>3.0000000000000004</v>
-      </c>
-      <c r="I28" s="14">
+        <v>3.75</v>
+      </c>
+      <c r="I29" s="14">
         <f t="shared" si="2"/>
-        <v>41.88</v>
-      </c>
-      <c r="J28" s="14">
+        <v>51.879999999999995</v>
+      </c>
+      <c r="J29" s="14">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="K28" s="14">
+      <c r="K29" s="14">
         <f t="shared" si="2"/>
         <v>15.082352941176469</v>
       </c>
-      <c r="L28" s="14">
+      <c r="L29" s="14">
         <f t="shared" si="2"/>
-        <v>12.000000000000002</v>
-      </c>
-      <c r="M28" s="15">
+        <v>15</v>
+      </c>
+      <c r="M29" s="15">
         <f t="shared" si="2"/>
-        <v>3.0000000000000004</v>
-      </c>
-      <c r="N28" s="10">
-        <f>SUM(C28:M28)</f>
-        <v>104.04553529411764</v>
+        <v>3.75</v>
+      </c>
+      <c r="N29" s="10">
+        <f>SUM(C29:M29)</f>
+        <v>120.78765294117646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>